<commit_message>
Fixed mistake in Clouds BOM
</commit_message>
<xml_diff>
--- a/clouds/hardware_design/Clouds.xlsx
+++ b/clouds/hardware_design/Clouds.xlsx
@@ -513,9 +513,6 @@
     <t>LED1, LED2, LED3, LED4</t>
   </si>
   <si>
-    <t>LED 5mm, red &amp; green, diffused, common anode</t>
-  </si>
-  <si>
     <t>604-WP59EGW</t>
   </si>
   <si>
@@ -655,6 +652,9 @@
   </si>
   <si>
     <t>Texas Instruments CD74HC595M, NXP 74HC595D,112</t>
+  </si>
+  <si>
+    <t>LED 5mm, red &amp; green, diffused, common K</t>
   </si>
 </sst>
 </file>
@@ -1293,7 +1293,7 @@
   <dimension ref="A1:AMJ56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1313,7 +1313,7 @@
   <sheetData>
     <row r="1" spans="1:1024" ht="29" customHeight="1">
       <c r="A1" s="31" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
@@ -9680,13 +9680,13 @@
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F12" s="24" t="s">
         <v>15</v>
       </c>
       <c r="G12" s="23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H12" s="23"/>
       <c r="I12" s="23"/>
@@ -9958,7 +9958,7 @@
     </row>
     <row r="20" spans="1:1024" s="26" customFormat="1">
       <c r="A20" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B20" s="23">
         <v>6</v>
@@ -10017,7 +10017,7 @@
         <v>63</v>
       </c>
       <c r="H21" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I21" s="23"/>
       <c r="J21" s="25"/>
@@ -10116,7 +10116,7 @@
     </row>
     <row r="24" spans="1:1024" s="26" customFormat="1">
       <c r="A24" s="23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B24" s="23">
         <v>2</v>
@@ -10196,7 +10196,7 @@
     </row>
     <row r="26" spans="1:1024" s="26" customFormat="1">
       <c r="A26" s="23" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B26" s="23">
         <v>6</v>
@@ -10236,7 +10236,7 @@
     </row>
     <row r="27" spans="1:1024" s="26" customFormat="1">
       <c r="A27" s="23" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B27" s="23">
         <v>2</v>
@@ -10251,13 +10251,13 @@
         <v>84</v>
       </c>
       <c r="F27" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="G27" s="27" t="s">
         <v>187</v>
       </c>
-      <c r="G27" s="27" t="s">
+      <c r="H27" s="25" t="s">
         <v>188</v>
-      </c>
-      <c r="H27" s="25" t="s">
-        <v>189</v>
       </c>
       <c r="I27" s="23"/>
       <c r="J27" s="28"/>
@@ -10363,7 +10363,7 @@
         <v>102</v>
       </c>
       <c r="H30" s="23" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J30" s="25"/>
       <c r="K30" s="25"/>
@@ -10638,7 +10638,7 @@
         <v>2</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D38" s="29"/>
       <c r="E38" s="29"/>
@@ -10646,10 +10646,10 @@
         <v>111</v>
       </c>
       <c r="G38" s="29" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H38" s="23" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J38" s="25"/>
       <c r="K38" s="25"/>
@@ -10730,13 +10730,13 @@
     </row>
     <row r="41" spans="1:1024" s="26" customFormat="1">
       <c r="A41" s="23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B41" s="23">
         <v>1</v>
       </c>
       <c r="C41" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D41" s="23"/>
       <c r="E41" s="30"/>
@@ -10744,10 +10744,10 @@
         <v>147</v>
       </c>
       <c r="G41" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="H41" s="23" t="s">
         <v>196</v>
-      </c>
-      <c r="H41" s="23" t="s">
-        <v>197</v>
       </c>
       <c r="I41" s="23"/>
       <c r="J41" s="25"/>
@@ -10782,7 +10782,7 @@
         <v>153</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J42" s="21"/>
       <c r="K42" s="21"/>
@@ -12865,7 +12865,7 @@
         <v>160</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J45" s="21"/>
       <c r="K45" s="21"/>
@@ -12893,7 +12893,7 @@
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="H46" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J46" s="21"/>
       <c r="K46" s="21"/>
@@ -13918,15 +13918,15 @@
         <v>4</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>164</v>
+        <v>211</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="H47" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>166</v>
       </c>
       <c r="J47" s="21"/>
       <c r="K47" s="21"/>
@@ -14945,18 +14945,18 @@
     </row>
     <row r="48" spans="1:1024">
       <c r="A48" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B48" s="1">
         <v>1</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="H48" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J48" s="21"/>
       <c r="K48" s="21"/>
@@ -15975,21 +15975,21 @@
     </row>
     <row r="49" spans="1:1023">
       <c r="A49" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B49" s="1">
         <v>2</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="H49" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="J49" s="21"/>
       <c r="K49" s="21"/>
@@ -17008,21 +17008,21 @@
     </row>
     <row r="50" spans="1:1023">
       <c r="A50" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B50" s="1">
         <v>2</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="H50" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>175</v>
       </c>
       <c r="J50" s="21"/>
       <c r="K50" s="21"/>
@@ -18041,7 +18041,7 @@
     </row>
     <row r="51" spans="1:1023">
       <c r="A51" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B51" s="12"/>
       <c r="C51" s="11"/>
@@ -19068,16 +19068,16 @@
     </row>
     <row r="52" spans="1:1023" s="1" customFormat="1" ht="11">
       <c r="A52" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B52" s="1">
         <v>1</v>
       </c>
       <c r="C52" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G52" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="J52" s="21"/>
       <c r="K52" s="21"/>
@@ -19094,16 +19094,16 @@
     </row>
     <row r="53" spans="1:1023" s="1" customFormat="1" ht="11">
       <c r="A53" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B53" s="1">
         <v>1</v>
       </c>
       <c r="C53" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G53" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="J53" s="21"/>
       <c r="K53" s="21"/>
@@ -19120,16 +19120,16 @@
     </row>
     <row r="54" spans="1:1023" s="1" customFormat="1" ht="11">
       <c r="A54" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B54" s="1">
         <v>1</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="G54" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="J54" s="21"/>
       <c r="K54" s="21"/>
@@ -19146,7 +19146,7 @@
     </row>
     <row r="55" spans="1:1023">
       <c r="A55" s="11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="11"/>
@@ -20173,11 +20173,11 @@
     </row>
     <row r="56" spans="1:1023">
       <c r="A56" s="15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B56" s="16"/>
       <c r="C56" s="15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D56" s="15"/>
       <c r="E56" s="17"/>

</xml_diff>